<commit_message>
extraction des eleves ayant plus de 20ans
</commit_message>
<xml_diff>
--- a/ProjetDATASCIENCE.xlsx
+++ b/ProjetDATASCIENCE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="187">
   <si>
     <t xml:space="preserve">NOM</t>
   </si>
@@ -55,9 +55,6 @@
     <t xml:space="preserve">Keur Massar</t>
   </si>
   <si>
-    <t xml:space="preserve">18 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kaolack</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t xml:space="preserve">Médina</t>
   </si>
   <si>
-    <t xml:space="preserve">30 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dakar</t>
   </si>
   <si>
@@ -97,9 +91,6 @@
     <t xml:space="preserve">Parcelles</t>
   </si>
   <si>
-    <t xml:space="preserve">29 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">science naturelle</t>
   </si>
   <si>
@@ -112,9 +103,6 @@
     <t xml:space="preserve">Pikine</t>
   </si>
   <si>
-    <t xml:space="preserve">16 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ziguichor</t>
   </si>
   <si>
@@ -157,9 +145,6 @@
     <t xml:space="preserve">Liberté 6</t>
   </si>
   <si>
-    <t xml:space="preserve">15 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sociologie</t>
   </si>
   <si>
@@ -181,9 +166,6 @@
     <t xml:space="preserve">Almady</t>
   </si>
   <si>
-    <t xml:space="preserve">22 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Louga</t>
   </si>
   <si>
@@ -205,9 +187,6 @@
     <t xml:space="preserve">Rufisque</t>
   </si>
   <si>
-    <t xml:space="preserve">25 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tamba</t>
   </si>
   <si>
@@ -223,9 +202,6 @@
     <t xml:space="preserve">Diamniadio</t>
   </si>
   <si>
-    <t xml:space="preserve">19 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kaffrine</t>
   </si>
   <si>
@@ -241,9 +217,6 @@
     <t xml:space="preserve">Diass</t>
   </si>
   <si>
-    <t xml:space="preserve">26 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Topographie</t>
   </si>
   <si>
@@ -253,9 +226,6 @@
     <t xml:space="preserve">Malika</t>
   </si>
   <si>
-    <t xml:space="preserve">20 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Statistique</t>
   </si>
   <si>
@@ -268,9 +238,6 @@
     <t xml:space="preserve">Thiaroye</t>
   </si>
   <si>
-    <t xml:space="preserve">23 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kaoalck</t>
   </si>
   <si>
@@ -286,9 +253,6 @@
     <t xml:space="preserve">Niary Taly</t>
   </si>
   <si>
-    <t xml:space="preserve">31 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Matam</t>
   </si>
   <si>
@@ -304,9 +268,6 @@
     <t xml:space="preserve"> Biscuiterie</t>
   </si>
   <si>
-    <t xml:space="preserve">21 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Saint-Louis</t>
   </si>
   <si>
@@ -319,9 +280,6 @@
     <t xml:space="preserve">Marguerite</t>
   </si>
   <si>
-    <t xml:space="preserve">35 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">logistique</t>
   </si>
   <si>
@@ -337,9 +295,6 @@
     <t xml:space="preserve">Mantoulaye</t>
   </si>
   <si>
-    <t xml:space="preserve">37 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sène</t>
   </si>
   <si>
@@ -367,9 +322,6 @@
     <t xml:space="preserve">El Hadji</t>
   </si>
   <si>
-    <t xml:space="preserve">24 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kédougou</t>
   </si>
   <si>
@@ -442,15 +394,9 @@
     <t xml:space="preserve">Kébé</t>
   </si>
   <si>
-    <t xml:space="preserve">Mansour</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tobago</t>
   </si>
   <si>
-    <t xml:space="preserve">27 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mbow</t>
   </si>
   <si>
@@ -475,9 +421,6 @@
     <t xml:space="preserve">Awa</t>
   </si>
   <si>
-    <t xml:space="preserve">32 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yaly</t>
   </si>
   <si>
@@ -490,9 +433,6 @@
     <t xml:space="preserve">Moustapha</t>
   </si>
   <si>
-    <t xml:space="preserve">34 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">tamba</t>
   </si>
   <si>
@@ -511,9 +451,6 @@
     <t xml:space="preserve">Lamine</t>
   </si>
   <si>
-    <t xml:space="preserve">33 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comptabilité</t>
   </si>
   <si>
@@ -532,9 +469,6 @@
     <t xml:space="preserve">Yacine</t>
   </si>
   <si>
-    <t xml:space="preserve">38 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Aissatou</t>
   </si>
   <si>
@@ -550,9 +484,6 @@
     <t xml:space="preserve">Grand Médine</t>
   </si>
   <si>
-    <t xml:space="preserve">39 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bocar</t>
   </si>
   <si>
@@ -586,27 +517,18 @@
     <t xml:space="preserve">Osama</t>
   </si>
   <si>
-    <t xml:space="preserve">17 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dasylva</t>
   </si>
   <si>
     <t xml:space="preserve">Sylvie</t>
   </si>
   <si>
-    <t xml:space="preserve">13 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Derneville</t>
   </si>
   <si>
     <t xml:space="preserve">Ange</t>
   </si>
   <si>
-    <t xml:space="preserve">14 ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ndiath</t>
   </si>
   <si>
@@ -623,9 +545,6 @@
   </si>
   <si>
     <t xml:space="preserve">Mouhamed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 ans</t>
   </si>
   <si>
     <t xml:space="preserve">Souleymane</t>
@@ -796,7 +715,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -851,571 +770,571 @@
       <c r="D2" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>25</v>
+      <c r="E4" s="2" t="n">
+        <v>29</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>14.5</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>30</v>
+      <c r="E5" s="2" t="n">
+        <v>16</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
+      <c r="E6" s="2" t="n">
+        <v>18</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>30</v>
+      <c r="E7" s="2" t="n">
+        <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>13.75</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>45</v>
+      <c r="E8" s="2" t="n">
+        <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>18</v>
+      <c r="E9" s="2" t="n">
+        <v>30</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>53</v>
+      <c r="E10" s="2" t="n">
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>16.5</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>11</v>
+      <c r="E11" s="2" t="n">
+        <v>18</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>61</v>
+      <c r="E12" s="2" t="n">
+        <v>25</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>67</v>
+      <c r="E13" s="2" t="n">
+        <v>19</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>73</v>
+      <c r="E14" s="2" t="n">
+        <v>26</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>77</v>
+      <c r="E15" s="2" t="n">
+        <v>20</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>3.5</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>82</v>
+      <c r="E16" s="2" t="n">
+        <v>23</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>56</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>88</v>
+      <c r="E17" s="2" t="n">
+        <v>31</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D18" s="2" t="n">
         <v>10.5</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>94</v>
+      <c r="E18" s="2" t="n">
+        <v>21</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D19" s="2" t="n">
         <v>11.5</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>99</v>
+      <c r="E19" s="2" t="n">
+        <v>35</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D20" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>82</v>
+      <c r="E20" s="2" t="n">
+        <v>23</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D21" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>105</v>
+      <c r="E21" s="2" t="n">
+        <v>37</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D22" s="2" t="n">
         <v>19.5</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>73</v>
+      <c r="E22" s="2" t="n">
+        <v>26</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>45</v>
+      <c r="E23" s="2" t="n">
+        <v>15</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>10</v>
@@ -1423,337 +1342,335 @@
       <c r="D24" s="2" t="n">
         <v>15.5</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>115</v>
+      <c r="E24" s="2" t="n">
+        <v>24</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D25" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>88</v>
+      <c r="E25" s="2" t="n">
+        <v>31</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D26" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>11</v>
+      <c r="E26" s="2" t="n">
+        <v>18</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D27" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>61</v>
+      <c r="E27" s="2" t="n">
+        <v>25</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D28" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>88</v>
+      <c r="E28" s="2" t="n">
+        <v>31</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D29" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>67</v>
+      <c r="E29" s="2" t="n">
+        <v>19</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="D30" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>53</v>
+      <c r="E30" s="2" t="n">
+        <v>22</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="D31" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>82</v>
+      <c r="E31" s="2" t="n">
+        <v>23</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="D32" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>67</v>
+      <c r="E32" s="2" t="n">
+        <v>19</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>140</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="D33" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>142</v>
+      <c r="E33" s="2" t="n">
+        <v>27</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="D34" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H34" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="D35" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>73</v>
+      <c r="E35" s="2" t="n">
+        <v>26</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D36" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>151</v>
+      <c r="E36" s="2" t="n">
+        <v>32</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>10</v>
@@ -1761,589 +1678,589 @@
       <c r="D37" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>142</v>
+      <c r="E37" s="2" t="n">
+        <v>27</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D38" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>156</v>
+      <c r="E38" s="2" t="n">
+        <v>34</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D39" s="2" t="n">
         <v>10.5</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>11</v>
+      <c r="E39" s="2" t="n">
+        <v>18</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D40" s="2" t="n">
         <v>13.75</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>163</v>
+      <c r="E40" s="2" t="n">
+        <v>33</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="D41" s="2" t="n">
         <v>19.5</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>30</v>
+      <c r="E41" s="2" t="n">
+        <v>16</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D42" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>170</v>
+      <c r="E42" s="2" t="n">
+        <v>38</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D43" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>73</v>
+      <c r="E43" s="2" t="n">
+        <v>26</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="D44" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>176</v>
+      <c r="E44" s="2" t="n">
+        <v>39</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="D45" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>45</v>
+      <c r="E45" s="2" t="n">
+        <v>15</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="D46" s="2" t="n">
         <v>12.5</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>11</v>
+      <c r="E46" s="2" t="n">
+        <v>18</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="D47" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>82</v>
+      <c r="E47" s="2" t="n">
+        <v>23</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="D48" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>188</v>
+      <c r="E48" s="2" t="n">
+        <v>17</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D49" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>191</v>
+      <c r="E49" s="2" t="n">
+        <v>13</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D50" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>194</v>
+      <c r="E50" s="2" t="n">
+        <v>14</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="D51" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>25</v>
+      <c r="E51" s="2" t="n">
+        <v>29</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="D52" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>67</v>
+      <c r="E52" s="2" t="n">
+        <v>19</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D53" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>201</v>
+      <c r="E53" s="2" t="n">
+        <v>28</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>202</v>
+        <v>175</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D54" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>191</v>
+      <c r="E54" s="2" t="n">
+        <v>13</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>205</v>
+        <v>178</v>
       </c>
       <c r="D55" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>176</v>
+      <c r="E55" s="2" t="n">
+        <v>39</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="D56" s="2" t="n">
         <v>18.5</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>30</v>
+      <c r="E56" s="2" t="n">
+        <v>16</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
       <c r="D57" s="2" t="n">
         <v>10.75</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>67</v>
+      <c r="E57" s="2" t="n">
+        <v>19</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>211</v>
+        <v>184</v>
       </c>
       <c r="D58" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>11</v>
+      <c r="E58" s="2" t="n">
+        <v>18</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>212</v>
+        <v>185</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>213</v>
+        <v>186</v>
       </c>
       <c r="D59" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>188</v>
+      <c r="E59" s="2" t="n">
+        <v>17</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>